<commit_message>
feat: [Eng] Adding more content about the first exam
</commit_message>
<xml_diff>
--- a/Engenharia_bioquimica_1/Linearização/EB1 (1).xlsx
+++ b/Engenharia_bioquimica_1/Linearização/EB1 (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Isaac\Faculdade\Quimica\EQ_github\Engenharia_bioquimica_1\Linearização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E0AD1-9BF1-4ED5-9E55-B79E96BC228B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E432E60-1CB9-457A-9D61-C60C6DCAE50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11835" xr2:uid="{766D9221-9E2B-4246-A691-92AAEA63C218}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{766D9221-9E2B-4246-A691-92AAEA63C218}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -433,19 +433,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2500000000000001E-2</c:v>
+                  <c:v>3.3333333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>1.4285714285714286E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,19 +457,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.8809946714031973</c:v>
+                  <c:v>3.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8449612403100772</c:v>
+                  <c:v>1.9193857965451055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6166365280289328</c:v>
+                  <c:v>1.4306151645207441</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6101083032490973</c:v>
+                  <c:v>0.9009009009009008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3760972316002698</c:v>
+                  <c:v>0.75187969924812026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,19 +844,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2500000000000001E-2</c:v>
+                  <c:v>3.3333333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>1.4285714285714286E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -868,19 +868,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.8823529411764701</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3478260869565215</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4482758620689657</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6666666666666667</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3513513513513513</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1225,19 +1225,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,19 +1249,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>88.809946714031966</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>145.34883720930233</c:v>
+                  <c:v>95.969289827255281</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180.83182640144665</c:v>
+                  <c:v>143.06151645207441</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>288.80866425992775</c:v>
+                  <c:v>270.27027027027026</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>337.60972316002699</c:v>
+                  <c:v>526.31578947368416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3714,8 +3714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C8A947-D9C1-4D53-9581-FC0B97E60EE7}">
   <dimension ref="B10:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F15" zoomScale="104" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="107" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,177 +3872,177 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>0.11260000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="D17" s="1">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <f>1/B17</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G17" s="1">
         <f>1/C17</f>
-        <v>8.8809946714031973</v>
+        <v>3.125</v>
       </c>
       <c r="I17" s="1">
         <f>B17</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J17" s="1">
         <f>B17/C17</f>
-        <v>88.809946714031966</v>
+        <v>62.5</v>
       </c>
       <c r="L17" s="5">
         <f>1/J17</f>
-        <v>1.1260000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="M17" s="5">
         <f>C17</f>
-        <v>0.11260000000000001</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C18" s="3">
-        <v>0.2064</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="D18" s="1">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ref="F18:F27" si="0">1/B18</f>
-        <v>3.3333333333333333E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G27" si="1">1/C18</f>
-        <v>4.8449612403100772</v>
+        <v>1.9193857965451055</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" ref="I18:I27" si="2">B18</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" ref="J18:J27" si="3">B18/C18</f>
-        <v>145.34883720930233</v>
+        <v>95.969289827255281</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" ref="L18:L27" si="4">1/J18</f>
-        <v>6.8799999999999998E-3</v>
+        <v>1.042E-2</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" ref="M18:M27" si="5">C18</f>
-        <v>0.2064</v>
+        <v>0.52100000000000002</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C19" s="3">
-        <v>0.27650000000000002</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="D19" s="1">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
-        <v>3.6166365280289328</v>
+        <v>1.4306151645207441</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>180.83182640144665</v>
+        <v>143.06151645207441</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="4"/>
-        <v>5.5300000000000002E-3</v>
+        <v>6.9899999999999988E-3</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="5"/>
-        <v>0.27650000000000002</v>
+        <v>0.69899999999999995</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="C20" s="3">
-        <v>0.27700000000000002</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D20" s="1">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>1.2500000000000001E-2</v>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
-        <v>3.6101083032490973</v>
+        <v>0.9009009009009008</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>288.80866425992775</v>
+        <v>270.27027027027026</v>
       </c>
       <c r="L20" s="5">
         <f t="shared" si="4"/>
-        <v>3.4625000000000007E-3</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>0.27700000000000002</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="C21" s="3">
-        <v>0.29620000000000002</v>
+        <v>1.33</v>
       </c>
       <c r="D21" s="1">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>1.4285714285714286E-3</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
-        <v>3.3760972316002698</v>
+        <v>0.75187969924812026</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>337.60972316002699</v>
+        <v>526.31578947368416</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="4"/>
-        <v>2.9620000000000002E-3</v>
+        <v>1.9000000000000002E-3</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>0.29620000000000002</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -4398,11 +4398,11 @@
     <row r="56" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F56" s="1">
         <f t="shared" ref="F56:F66" si="6">1/B17</f>
-        <v>0.1</v>
-      </c>
-      <c r="G56" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G56" s="1" t="e">
         <f t="shared" ref="G56:G66" si="7">1/D17</f>
-        <v>5.8823529411764701</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>0</v>
@@ -4420,105 +4420,105 @@
     <row r="57" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F57" s="1">
         <f t="shared" si="6"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G57" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G57" s="1" t="e">
         <f t="shared" si="7"/>
-        <v>4.3478260869565215</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" ref="I57:I67" si="8">1/B17</f>
-        <v>0.1</v>
-      </c>
-      <c r="J57" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J57" s="1" t="e">
         <f>1/D17</f>
-        <v>5.8823529411764701</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L57" s="1">
         <f t="shared" ref="L57:L67" si="9">1/B17</f>
-        <v>0.1</v>
-      </c>
-      <c r="M57" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M57" s="1" t="e">
         <f t="shared" ref="M57:M67" si="10">1/D17</f>
-        <v>5.8823529411764701</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="58" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F58" s="1">
         <f t="shared" si="6"/>
-        <v>0.02</v>
-      </c>
-      <c r="G58" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G58" s="1" t="e">
         <f t="shared" si="7"/>
-        <v>3.4482758620689657</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I58" s="1">
         <f t="shared" si="8"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="J58" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="J58" s="1" t="e">
         <f t="shared" ref="J58:J67" si="11">1/D18</f>
-        <v>4.3478260869565215</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" si="9"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="M58" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M58" s="1" t="e">
         <f t="shared" si="10"/>
-        <v>4.3478260869565215</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="59" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F59" s="1">
         <f t="shared" si="6"/>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="G59" s="1">
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="G59" s="1" t="e">
         <f t="shared" si="7"/>
-        <v>1.6666666666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I59" s="1">
         <f t="shared" si="8"/>
-        <v>0.02</v>
-      </c>
-      <c r="J59" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J59" s="1" t="e">
         <f t="shared" si="11"/>
-        <v>3.4482758620689657</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L59" s="1">
         <f t="shared" si="9"/>
-        <v>0.02</v>
-      </c>
-      <c r="M59" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M59" s="1" t="e">
         <f t="shared" si="10"/>
-        <v>3.4482758620689657</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="60" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F60" s="1">
         <f t="shared" si="6"/>
-        <v>0.01</v>
-      </c>
-      <c r="G60" s="1">
+        <v>1.4285714285714286E-3</v>
+      </c>
+      <c r="G60" s="1" t="e">
         <f t="shared" si="7"/>
-        <v>1.3513513513513513</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" si="8"/>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="J60" s="1">
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="J60" s="1" t="e">
         <f t="shared" si="11"/>
-        <v>1.6666666666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" si="9"/>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="M60" s="1">
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="M60" s="1" t="e">
         <f t="shared" si="10"/>
-        <v>1.6666666666666667</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="6:13" x14ac:dyDescent="0.25">
@@ -4532,19 +4532,19 @@
       </c>
       <c r="I61" s="1">
         <f t="shared" si="8"/>
-        <v>0.01</v>
-      </c>
-      <c r="J61" s="1">
+        <v>1.4285714285714286E-3</v>
+      </c>
+      <c r="J61" s="1" t="e">
         <f t="shared" si="11"/>
-        <v>1.3513513513513513</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" si="9"/>
-        <v>0.01</v>
-      </c>
-      <c r="M61" s="1">
+        <v>1.4285714285714286E-3</v>
+      </c>
+      <c r="M61" s="1" t="e">
         <f t="shared" si="10"/>
-        <v>1.3513513513513513</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="62" spans="6:13" x14ac:dyDescent="0.25">

</xml_diff>